<commit_message>
Added code to calculate average
</commit_message>
<xml_diff>
--- a/new_output.xlsx
+++ b/new_output.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="283">
   <si>
     <t>study_id</t>
   </si>
   <si>
-    <t>ActualEnrollment</t>
-  </si>
-  <si>
-    <t>OriginalEnrollment</t>
+    <t>ActualEnrollment Avg: 289.31</t>
+  </si>
+  <si>
+    <t>OriginalEnrollment Avg: 265.53</t>
   </si>
   <si>
     <t>StudyStartDate</t>
@@ -43,15 +43,27 @@
     <t>difference</t>
   </si>
   <si>
+    <t>NCT05297565</t>
+  </si>
+  <si>
     <t>NCT05621148</t>
   </si>
   <si>
-    <t>NCT05297565</t>
+    <t>NCT03829722</t>
   </si>
   <si>
     <t>NCT03502330</t>
   </si>
   <si>
+    <t>NCT04570839</t>
+  </si>
+  <si>
+    <t>NCT05952089</t>
+  </si>
+  <si>
+    <t>NCT04766892</t>
+  </si>
+  <si>
     <t>NCT06361576</t>
   </si>
   <si>
@@ -61,135 +73,144 @@
     <t>NCT05498480</t>
   </si>
   <si>
+    <t>NCT04513522</t>
+  </si>
+  <si>
+    <t>NCT06361563</t>
+  </si>
+  <si>
+    <t>NCT03583086</t>
+  </si>
+  <si>
+    <t>NCT03667716</t>
+  </si>
+  <si>
+    <t>NCT04349072</t>
+  </si>
+  <si>
+    <t>NCT04124601</t>
+  </si>
+  <si>
+    <t>NCT04736134</t>
+  </si>
+  <si>
+    <t>NCT02913313</t>
+  </si>
+  <si>
+    <t>NCT02927769</t>
+  </si>
+  <si>
     <t>NCT02464969</t>
   </si>
   <si>
-    <t>NCT03667716</t>
+    <t>NCT02553642</t>
+  </si>
+  <si>
+    <t>NCT03970252</t>
   </si>
   <si>
     <t>NCT02872116</t>
   </si>
   <si>
-    <t>NCT04513522</t>
-  </si>
-  <si>
-    <t>NCT03829722</t>
-  </si>
-  <si>
-    <t>NCT04570839</t>
-  </si>
-  <si>
-    <t>NCT06361563</t>
-  </si>
-  <si>
-    <t>NCT04736134</t>
-  </si>
-  <si>
-    <t>NCT04766892</t>
-  </si>
-  <si>
-    <t>NCT04349072</t>
-  </si>
-  <si>
-    <t>NCT04124601</t>
-  </si>
-  <si>
-    <t>NCT05952089</t>
+    <t>NCT05901714</t>
+  </si>
+  <si>
+    <t>NCT05838781</t>
+  </si>
+  <si>
+    <t>NCT04161781</t>
+  </si>
+  <si>
+    <t>NCT03138512</t>
   </si>
   <si>
     <t>NCT04197310</t>
   </si>
   <si>
-    <t>NCT04161781</t>
-  </si>
-  <si>
-    <t>NCT02927769</t>
-  </si>
-  <si>
-    <t>NCT02913313</t>
+    <t>NCT02375555</t>
+  </si>
+  <si>
+    <t>NCT01471106</t>
+  </si>
+  <si>
+    <t>NCT03662659</t>
+  </si>
+  <si>
+    <t>NCT04282109</t>
+  </si>
+  <si>
+    <t>NCT02576509</t>
+  </si>
+  <si>
+    <t>NCT05025085</t>
+  </si>
+  <si>
+    <t>NCT03195478</t>
+  </si>
+  <si>
+    <t>NCT03161379</t>
   </si>
   <si>
     <t>NCT03712943</t>
   </si>
   <si>
-    <t>NCT05838781</t>
-  </si>
-  <si>
-    <t>NCT05901714</t>
-  </si>
-  <si>
-    <t>NCT03138512</t>
-  </si>
-  <si>
-    <t>NCT03970252</t>
-  </si>
-  <si>
-    <t>NCT02553642</t>
-  </si>
-  <si>
-    <t>NCT01471106</t>
-  </si>
-  <si>
     <t>NCT01954979</t>
   </si>
   <si>
-    <t>NCT03161379</t>
-  </si>
-  <si>
-    <t>NCT03662659</t>
+    <t>NCT03558087</t>
+  </si>
+  <si>
+    <t>NCT02847728</t>
+  </si>
+  <si>
+    <t>NCT06084598</t>
+  </si>
+  <si>
+    <t>NCT03635983</t>
+  </si>
+  <si>
+    <t>NCT01844505</t>
+  </si>
+  <si>
+    <t>NCT04540705</t>
+  </si>
+  <si>
+    <t>NCT03241745</t>
+  </si>
+  <si>
+    <t>NCT02667587</t>
   </si>
   <si>
     <t>NCT04698187</t>
   </si>
   <si>
-    <t>NCT05025085</t>
-  </si>
-  <si>
-    <t>NCT03195478</t>
+    <t>NCT05064787</t>
   </si>
   <si>
     <t>NCT04704154</t>
   </si>
   <si>
-    <t>NCT03558087</t>
-  </si>
-  <si>
-    <t>NCT02667587</t>
-  </si>
-  <si>
-    <t>NCT02576509</t>
-  </si>
-  <si>
-    <t>NCT05064787</t>
-  </si>
-  <si>
-    <t>NCT03635983</t>
-  </si>
-  <si>
-    <t>NCT02847728</t>
-  </si>
-  <si>
-    <t>NCT01844505</t>
-  </si>
-  <si>
-    <t>NCT04540705</t>
-  </si>
-  <si>
-    <t>NCT06084598</t>
-  </si>
-  <si>
-    <t>NCT03241745</t>
+    <t>14</t>
   </si>
   <si>
     <t>152</t>
   </si>
   <si>
-    <t>14</t>
+    <t>26</t>
   </si>
   <si>
     <t>42</t>
   </si>
   <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>700</t>
   </si>
   <si>
@@ -199,115 +220,115 @@
     <t>6</t>
   </si>
   <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
     <t>229</t>
   </si>
   <si>
-    <t>121</t>
+    <t>81</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
   <si>
     <t>2031</t>
   </si>
   <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>13</t>
+    <t>65</t>
+  </si>
+  <si>
+    <t>2112</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1653</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>72</t>
+    <t>40</t>
+  </si>
+  <si>
+    <t>274</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>743</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>36</t>
   </si>
   <si>
     <t>52</t>
   </si>
   <si>
-    <t>2112</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>1653</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
     <t>56</t>
   </si>
   <si>
-    <t>274</t>
+    <t>76</t>
+  </si>
+  <si>
+    <t>1189</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>783</t>
+  </si>
+  <si>
+    <t>1296</t>
+  </si>
+  <si>
+    <t>716</t>
   </si>
   <si>
     <t>44</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>36</t>
+    <t>45</t>
   </si>
   <si>
     <t>175</t>
   </si>
   <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>716</t>
-  </si>
-  <si>
-    <t>743</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>783</t>
-  </si>
-  <si>
-    <t>1189</t>
-  </si>
-  <si>
-    <t>1296</t>
-  </si>
-  <si>
-    <t>24</t>
+    <t>286</t>
   </si>
   <si>
     <t>120</t>
   </si>
   <si>
-    <t>286</t>
+    <t>100</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
   <si>
     <t>Same as current</t>
@@ -319,78 +340,81 @@
     <t>12</t>
   </si>
   <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
     <t>150</t>
   </si>
   <si>
-    <t>140</t>
-  </si>
-  <si>
     <t>750</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>170</t>
+    <t>50</t>
   </si>
   <si>
     <t>2960</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>800</t>
   </si>
   <si>
     <t>300</t>
   </si>
   <si>
+    <t>726</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
     <t>22</t>
   </si>
   <si>
-    <t>27</t>
+    <t>63</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>764</t>
+  </si>
+  <si>
+    <t>915</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>320</t>
   </si>
   <si>
     <t>200</t>
   </si>
   <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>320</t>
-  </si>
-  <si>
-    <t>726</t>
-  </si>
-  <si>
-    <t>764</t>
-  </si>
-  <si>
-    <t>1200</t>
-  </si>
-  <si>
-    <t>915</t>
-  </si>
-  <si>
-    <t>104</t>
+    <t>2022-08-03</t>
   </si>
   <si>
     <t>2023-01-25</t>
   </si>
   <si>
-    <t>2022-08-03</t>
+    <t>2019-09-05</t>
   </si>
   <si>
     <t>2018-06-09</t>
   </si>
   <si>
+    <t>2020-08-31</t>
+  </si>
+  <si>
+    <t>2023-08-17</t>
+  </si>
+  <si>
+    <t>2021-03-30</t>
+  </si>
+  <si>
     <t>2023-09-05</t>
   </si>
   <si>
@@ -400,132 +424,138 @@
     <t>2022-07-27</t>
   </si>
   <si>
+    <t>2020-12-17</t>
+  </si>
+  <si>
+    <t>2018-07-10</t>
+  </si>
+  <si>
+    <t>2018-09-06</t>
+  </si>
+  <si>
+    <t>2020-07-06</t>
+  </si>
+  <si>
+    <t>2020-06-01</t>
+  </si>
+  <si>
+    <t>2021-03-03</t>
+  </si>
+  <si>
+    <t>2016-11-30</t>
+  </si>
+  <si>
+    <t>2017-03-28</t>
+  </si>
+  <si>
     <t>2015-11-22</t>
   </si>
   <si>
-    <t>2018-09-06</t>
+    <t>2015-09-14</t>
+  </si>
+  <si>
+    <t>2019-07-24</t>
   </si>
   <si>
     <t>2016-10-12</t>
   </si>
   <si>
-    <t>2020-12-17</t>
-  </si>
-  <si>
-    <t>2019-09-05</t>
-  </si>
-  <si>
-    <t>2020-08-31</t>
-  </si>
-  <si>
-    <t>2021-03-03</t>
-  </si>
-  <si>
-    <t>2021-03-30</t>
-  </si>
-  <si>
-    <t>2020-07-06</t>
-  </si>
-  <si>
-    <t>2020-06-01</t>
-  </si>
-  <si>
-    <t>2023-08-17</t>
+    <t>2023-06-14</t>
+  </si>
+  <si>
+    <t>2023-12-04</t>
+  </si>
+  <si>
+    <t>2019-11-12</t>
+  </si>
+  <si>
+    <t>2017-07-07</t>
   </si>
   <si>
     <t>2019-12-26</t>
   </si>
   <si>
-    <t>2019-11-12</t>
-  </si>
-  <si>
-    <t>2017-03-28</t>
-  </si>
-  <si>
-    <t>2016-11-30</t>
+    <t>2015-05-07</t>
+  </si>
+  <si>
+    <t>2014-01-21</t>
+  </si>
+  <si>
+    <t>2018-10-16</t>
+  </si>
+  <si>
+    <t>2020-06-03</t>
+  </si>
+  <si>
+    <t>2015-12-07</t>
+  </si>
+  <si>
+    <t>2021-10-04</t>
+  </si>
+  <si>
+    <t>2017-08-02</t>
+  </si>
+  <si>
+    <t>2018-02-02</t>
   </si>
   <si>
     <t>2018-10-23</t>
   </si>
   <si>
-    <t>2023-12-04</t>
-  </si>
-  <si>
-    <t>2023-06-14</t>
-  </si>
-  <si>
-    <t>2017-07-07</t>
-  </si>
-  <si>
-    <t>2019-07-24</t>
-  </si>
-  <si>
-    <t>2015-09-14</t>
-  </si>
-  <si>
-    <t>2014-01-21</t>
-  </si>
-  <si>
     <t>2014-03-27</t>
   </si>
   <si>
-    <t>2018-02-02</t>
-  </si>
-  <si>
-    <t>2018-10-16</t>
+    <t>2018-07-13</t>
+  </si>
+  <si>
+    <t>2016-07-28</t>
+  </si>
+  <si>
+    <t>2023-10-12</t>
+  </si>
+  <si>
+    <t>2018-09-21</t>
+  </si>
+  <si>
+    <t>2013-06-11</t>
+  </si>
+  <si>
+    <t>2020-09-11</t>
+  </si>
+  <si>
+    <t>2017-08-03</t>
+  </si>
+  <si>
+    <t>2016-05-09</t>
   </si>
   <si>
     <t>2021-03-11</t>
   </si>
   <si>
-    <t>2021-10-04</t>
-  </si>
-  <si>
-    <t>2017-08-02</t>
+    <t>2022-03-11</t>
   </si>
   <si>
     <t>2021-02-03</t>
   </si>
   <si>
-    <t>2018-07-13</t>
-  </si>
-  <si>
-    <t>2016-05-09</t>
-  </si>
-  <si>
-    <t>2015-12-07</t>
-  </si>
-  <si>
-    <t>2022-03-11</t>
-  </si>
-  <si>
-    <t>2018-09-21</t>
-  </si>
-  <si>
-    <t>2016-07-28</t>
-  </si>
-  <si>
-    <t>2013-06-11</t>
-  </si>
-  <si>
-    <t>2020-09-11</t>
-  </si>
-  <si>
-    <t>2023-10-12</t>
-  </si>
-  <si>
-    <t>2017-08-03</t>
+    <t>2024-02-08</t>
   </si>
   <si>
     <t>2024-03-31</t>
   </si>
   <si>
-    <t>2024-02-08</t>
+    <t>2024-06-11</t>
   </si>
   <si>
     <t>2024-05-15</t>
   </si>
   <si>
+    <t>2024-03-19</t>
+  </si>
+  <si>
+    <t>2024-02-26</t>
+  </si>
+  <si>
     <t>2024-01-25</t>
   </si>
   <si>
@@ -535,103 +565,106 @@
     <t>2024-01-18</t>
   </si>
   <si>
+    <t>2024-01-04</t>
+  </si>
+  <si>
+    <t>2024-04-27</t>
+  </si>
+  <si>
+    <t>2024-01-30</t>
+  </si>
+  <si>
+    <t>2024-05-20</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
+    <t>2024-05-28</t>
+  </si>
+  <si>
     <t>2024-04-30</t>
   </si>
   <si>
-    <t>2024-01-30</t>
+    <t>2024-04-29</t>
+  </si>
+  <si>
+    <t>2024-05-25</t>
   </si>
   <si>
     <t>2024-06-06</t>
   </si>
   <si>
-    <t>2024-01-04</t>
-  </si>
-  <si>
-    <t>2024-06-11</t>
-  </si>
-  <si>
-    <t>2024-03-14</t>
-  </si>
-  <si>
-    <t>2024-02-26</t>
-  </si>
-  <si>
-    <t>2024-05-20</t>
-  </si>
-  <si>
-    <t>2024-03-15</t>
-  </si>
-  <si>
-    <t>2024-03-19</t>
+    <t>2024-04-11</t>
+  </si>
+  <si>
+    <t>2024-05-16</t>
+  </si>
+  <si>
+    <t>2024-03-06</t>
+  </si>
+  <si>
+    <t>2024-02-01</t>
   </si>
   <si>
     <t>2024-01-31</t>
   </si>
   <si>
-    <t>2024-03-06</t>
-  </si>
-  <si>
-    <t>2024-05-28</t>
-  </si>
-  <si>
-    <t>2024-05-16</t>
-  </si>
-  <si>
-    <t>2024-04-11</t>
-  </si>
-  <si>
-    <t>2024-02-01</t>
-  </si>
-  <si>
-    <t>2024-05-25</t>
-  </si>
-  <si>
-    <t>2024-04-29</t>
+    <t>2024-01-26</t>
   </si>
   <si>
     <t>2024-05-30</t>
   </si>
   <si>
+    <t>2024-03-21</t>
+  </si>
+  <si>
+    <t>2024-02-07</t>
+  </si>
+  <si>
+    <t>2024-04-01</t>
+  </si>
+  <si>
+    <t>2024-01-05</t>
+  </si>
+  <si>
+    <t>2024-02-28</t>
+  </si>
+  <si>
     <t>2024-01-16</t>
   </si>
   <si>
-    <t>2024-02-28</t>
+    <t>2024-03-07</t>
+  </si>
+  <si>
+    <t>2024-03-08</t>
+  </si>
+  <si>
+    <t>2024-04-19</t>
+  </si>
+  <si>
+    <t>2024-04-09</t>
   </si>
   <si>
     <t>2024-02-05</t>
   </si>
   <si>
-    <t>2024-04-01</t>
-  </si>
-  <si>
-    <t>2024-01-05</t>
+    <t>2024-02-06</t>
   </si>
   <si>
     <t>2024-03-29</t>
   </si>
   <si>
-    <t>2024-03-07</t>
-  </si>
-  <si>
-    <t>2024-04-09</t>
-  </si>
-  <si>
-    <t>2024-02-07</t>
-  </si>
-  <si>
-    <t>2024-02-06</t>
-  </si>
-  <si>
-    <t>2024-04-19</t>
-  </si>
-  <si>
-    <t>2024-03-08</t>
+    <t>Bristol-Myers Squibb</t>
   </si>
   <si>
     <t>French Innovative Leukemia Organisation</t>
   </si>
   <si>
-    <t>Bristol-Myers Squibb</t>
+    <t>University of Michigan Rogel Cancer Center</t>
   </si>
   <si>
     <t>Yale University</t>
@@ -640,100 +673,196 @@
     <t>Compugen Ltd</t>
   </si>
   <si>
-    <t>University of Michigan Rogel Cancer Center</t>
+    <t>Vanderbilt-Ingram Cancer Center</t>
   </si>
   <si>
     <t>Johannes Laengle, MD, PhD</t>
   </si>
   <si>
+    <t>Memorial Sloan Kettering Cancer Center</t>
+  </si>
+  <si>
+    <t>Jonsson Comprehensive Cancer Center</t>
+  </si>
+  <si>
     <t>Dana-Farber Cancer Institute</t>
   </si>
   <si>
-    <t>Memorial Sloan Kettering Cancer Center</t>
+    <t>M.D. Anderson Cancer Center</t>
+  </si>
+  <si>
+    <t>Grupo Español de Tratamiento de Tumores de Cabeza y Cuello</t>
+  </si>
+  <si>
+    <t>Sidney Kimmel Comprehensive Cancer Center at Johns Hopkins</t>
   </si>
   <si>
     <t>H. Lee Moffitt Cancer Center and Research Institute</t>
   </si>
   <si>
-    <t>Jonsson Comprehensive Cancer Center</t>
-  </si>
-  <si>
-    <t>M.D. Anderson Cancer Center</t>
-  </si>
-  <si>
     <t>Beth Israel Deaconess Medical Center</t>
   </si>
   <si>
-    <t>Sidney Kimmel Comprehensive Cancer Center at Johns Hopkins</t>
+    <t>Matthew Galsky</t>
   </si>
   <si>
     <t>Regeneron Pharmaceuticals</t>
   </si>
   <si>
+    <t>Pack Health</t>
+  </si>
+  <si>
     <t>Bayer</t>
   </si>
   <si>
-    <t>Matthew Galsky</t>
-  </si>
-  <si>
-    <t>Pack Health</t>
+    <t>MyoKardia, Inc.</t>
+  </si>
+  <si>
+    <t>Medical University of Vienna</t>
   </si>
   <si>
     <t>Pfizer</t>
   </si>
   <si>
-    <t>MyoKardia, Inc.</t>
-  </si>
-  <si>
-    <t>Medical University of Vienna</t>
+    <t>Agenus Inc.</t>
   </si>
   <si>
     <t>Checkmate Pharmaceuticals</t>
   </si>
   <si>
-    <t>Agenus Inc.</t>
-  </si>
-  <si>
     <t>Not provided</t>
   </si>
   <si>
     <t>Bristol-Myers SquibbApexigen America, Inc.National Cancer Institute (NCI)</t>
   </si>
   <si>
+    <t>Bristol-Myers SquibbXcovery Holdings, Inc.</t>
+  </si>
+  <si>
     <t>Ono Pharmaceutical Co. Ltd</t>
   </si>
   <si>
+    <t>Seagen Inc.</t>
+  </si>
+  <si>
+    <t>UConn HealthBristol-Myers SquibbAdaptive BiotechnologiesMedGenome</t>
+  </si>
+  <si>
+    <t>Bristol-Myers SquibbNovoCure Ltd.</t>
+  </si>
+  <si>
+    <t>Region HallandHalmstad UniversityKarolinska InstitutetPfizerPhilips Healthcare</t>
+  </si>
+  <si>
     <t>Bristol-Myers SquibbExelixis</t>
   </si>
   <si>
-    <t>Seagen Inc.</t>
-  </si>
-  <si>
-    <t>Region HallandHalmstad UniversityKarolinska InstitutetPfizerPhilips Healthcare</t>
-  </si>
-  <si>
-    <t>Bristol-Myers SquibbNovoCure Ltd.</t>
-  </si>
-  <si>
-    <t>UConn HealthBristol-Myers SquibbAdaptive BiotechnologiesMedGenome</t>
-  </si>
-  <si>
     <t>Susan G. Komen Breast Cancer FoundationBristol-Myers Squibb</t>
   </si>
   <si>
+    <t>Bristol-Myers SquibbApices Soluciones S.L.</t>
+  </si>
+  <si>
     <t>Bristol-Myers SquibbDana-Farber Cancer Institute</t>
   </si>
   <si>
+    <t>Bristol-Myers SquibbIcahn School of Medicine at Mount Sinai</t>
+  </si>
+  <si>
+    <t>Nektar Therapeutics</t>
+  </si>
+  <si>
+    <t>M.D. Anderson Cancer CenterBristol-Myers Squibb</t>
+  </si>
+  <si>
     <t>Bristol Myers Squibb Co. and Ono Pharmaceutical Co., Ltd</t>
   </si>
   <si>
-    <t>Bristol-Myers SquibbIcahn School of Medicine at Mount Sinai</t>
-  </si>
-  <si>
-    <t>M.D. Anderson Cancer CenterBristol-Myers Squibb</t>
-  </si>
-  <si>
-    <t>Nektar Therapeutics</t>
+    <t>272</t>
+  </si>
+  <si>
+    <t>-32</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>-12</t>
+  </si>
+  <si>
+    <t>-16</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>-79</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>-1281</t>
+  </si>
+  <si>
+    <t>-15</t>
+  </si>
+  <si>
+    <t>848</t>
+  </si>
+  <si>
+    <t>-853</t>
+  </si>
+  <si>
+    <t>-24</t>
+  </si>
+  <si>
+    <t>-17</t>
+  </si>
+  <si>
+    <t>-9</t>
+  </si>
+  <si>
+    <t>-34</t>
+  </si>
+  <si>
+    <t>-13</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>-19</t>
+  </si>
+  <si>
+    <t>-381</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>-396</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1235,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1149,28 +1278,28 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J2" s="3">
-        <v>32</v>
+        <v>238</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1181,28 +1310,28 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J3" s="4">
-        <v>-272</v>
+        <v>214</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1213,28 +1342,28 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="J4" s="4">
-        <v>-78</v>
+        <v>214</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1245,28 +1374,28 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0</v>
+        <v>239</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1277,28 +1406,28 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J6" s="4">
-        <v>-21</v>
+        <v>214</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1309,28 +1438,28 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J7" s="4">
-        <v>-6</v>
+        <v>238</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1341,28 +1470,28 @@
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="J8" s="3">
-        <v>79</v>
+        <v>238</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1373,28 +1502,28 @@
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J9" s="4">
-        <v>-19</v>
+        <v>238</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1405,28 +1534,28 @@
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J10" s="3">
-        <v>1281</v>
+        <v>238</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1437,28 +1566,28 @@
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J11" s="3">
-        <v>1</v>
+        <v>238</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1469,28 +1598,28 @@
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J12" s="4">
-        <v>-14</v>
+        <v>238</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1501,28 +1630,28 @@
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>133</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J13" s="4">
-        <v>-52</v>
+        <v>238</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1533,28 +1662,28 @@
         <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0</v>
+        <v>240</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1565,28 +1694,28 @@
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J15" s="3">
-        <v>16</v>
+        <v>214</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1597,28 +1726,28 @@
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J16" s="4">
-        <v>-5</v>
+        <v>238</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1629,28 +1758,28 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J17" s="3">
-        <v>12</v>
+        <v>214</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1661,28 +1790,28 @@
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>223</v>
+        <v>105</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0</v>
+        <v>238</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1693,28 +1822,28 @@
         <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J19" s="4">
-        <v>-3</v>
+        <v>241</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1725,28 +1854,28 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
+        <v>242</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1757,28 +1886,28 @@
         <v>28</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>98</v>
+        <v>235</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J21" s="4">
-        <v>-25</v>
+        <v>235</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1789,28 +1918,28 @@
         <v>29</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="J22" s="4">
-        <v>-8</v>
+        <v>243</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1821,28 +1950,28 @@
         <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J23" s="4">
-        <v>-69</v>
+        <v>244</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1853,28 +1982,28 @@
         <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J24" s="3">
-        <v>24</v>
+        <v>241</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1885,28 +2014,28 @@
         <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="J25" s="4">
-        <v>-848</v>
+        <v>238</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1917,28 +2046,28 @@
         <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J26" s="3">
-        <v>15</v>
+        <v>245</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1949,28 +2078,28 @@
         <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J27" s="3">
-        <v>853</v>
+        <v>214</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1981,28 +2110,28 @@
         <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J28" s="4">
-        <v>-8</v>
+        <v>238</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2013,28 +2142,28 @@
         <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J29" s="4">
-        <v>-39</v>
+        <v>246</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2045,28 +2174,28 @@
         <v>37</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J30" s="4">
-        <v>-274</v>
+        <v>214</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2077,28 +2206,28 @@
         <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="J31" s="3">
-        <v>34</v>
+        <v>247</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2109,28 +2238,28 @@
         <v>39</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J32" s="4">
-        <v>-22</v>
+        <v>238</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2141,28 +2270,28 @@
         <v>40</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J33" s="3">
-        <v>24</v>
+        <v>248</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2173,28 +2302,28 @@
         <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>224</v>
+        <v>105</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J34" s="4">
-        <v>-56</v>
+        <v>241</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2205,28 +2334,28 @@
         <v>42</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="J35" s="4">
-        <v>-50</v>
+        <v>236</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2237,28 +2366,28 @@
         <v>43</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J36" s="3">
-        <v>9</v>
+        <v>238</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2269,28 +2398,28 @@
         <v>44</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J37" s="4">
-        <v>-25</v>
+        <v>214</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2301,28 +2430,28 @@
         <v>45</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J38" s="3">
-        <v>13</v>
+        <v>214</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2333,28 +2462,28 @@
         <v>46</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J39" s="3">
-        <v>396</v>
+        <v>249</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2365,28 +2494,28 @@
         <v>47</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J40" s="3">
-        <v>17</v>
+        <v>250</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2397,28 +2526,28 @@
         <v>48</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="J41" s="4">
-        <v>-5</v>
+      <c r="J41" s="3" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2429,28 +2558,28 @@
         <v>49</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="J42" s="3">
-        <v>19</v>
+        <v>238</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2461,28 +2590,28 @@
         <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J43" s="4">
-        <v>-11</v>
+        <v>251</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2493,28 +2622,28 @@
         <v>51</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J44" s="3">
-        <v>381</v>
+        <v>238</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2525,28 +2654,28 @@
         <v>52</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="J45" s="4">
-        <v>-74</v>
+        <v>251</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2557,28 +2686,28 @@
         <v>53</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>203</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J46" s="3">
-        <v>0</v>
+        <v>214</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2589,28 +2718,124 @@
         <v>54</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J47" s="4">
-        <v>-5</v>
+      <c r="G48" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>